<commit_message>
typos essei dans description 5181ea0ef546a0d8a338989579e7881ae8624d5e
</commit_message>
<xml_diff>
--- a/ig/sd-typo-phase-3-et-4/ValueSet-eclaire-study-phase-vs.xlsx
+++ b/ig/sd-typo-phase-3-et-4/ValueSet-eclaire-study-phase-vs.xlsx
@@ -58,7 +58,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-15T13:38:36+00:00</t>
+    <t>2023-09-15T13:53:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -76,7 +76,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Value Set type de phase Eclaire de l'essei clinique.</t>
+    <t>Value Set type de phase Eclaire de l'essai clinique.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>